<commit_message>
Atualização da página de rosto
</commit_message>
<xml_diff>
--- a/Aprenda Excel Usando Excel.xlsx
+++ b/Aprenda Excel Usando Excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/Documents/GitHub/AprendaExcelUsandoExcel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5659683-18CB-7746-8C0B-039C5EADAC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A88C3A-48A5-4546-B455-6268BAC6D563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4640" yWindow="1840" windowWidth="28040" windowHeight="17440" xr2:uid="{BEAB5BE4-F684-DC48-92FB-55B2B06D943B}"/>
   </bookViews>
@@ -491,7 +491,7 @@
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="167" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="168" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="171" formatCode="[Red]0000000#"/>
+    <numFmt numFmtId="169" formatCode="[Red]0000000#"/>
   </numFmts>
   <fonts count="13">
     <font>
@@ -881,6 +881,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="22" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -899,18 +908,12 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="22" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -919,9 +922,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1442,16 +1442,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>452965</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>56444</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>311854</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>197555</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>395110</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>155223</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>338666</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1466,8 +1466,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13773854" y="1636888"/>
-          <a:ext cx="3272367" cy="2074335"/>
+          <a:off x="12800187" y="2370666"/>
+          <a:ext cx="5022146" cy="2370668"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1522,7 +1522,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Contato: henriquefb arroba gmail ponto com</a:t>
+            <a:t>Gostou? Foi útil pra vc? Alguma coisa não ficou clara? Tem algum feedback pra me dar? Eu adoraria conversar:</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1541,6 +1541,17 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
+            <a:t>email: henriquefb arroba gmail ponto com</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>Twitter: arroba henriquefb6</a:t>
           </a:r>
         </a:p>
@@ -1550,16 +1561,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>84667</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>14111</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>649111</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>762001</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>112890</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>14110</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>98779</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1574,8 +1585,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13405556" y="3965222"/>
-          <a:ext cx="4007556" cy="2074335"/>
+          <a:off x="13137444" y="5136444"/>
+          <a:ext cx="4360333" cy="2074335"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1623,87 +1634,6 @@
               </a:solidFill>
             </a:rPr>
             <a:t> pode ser distribuído livremente, desde que de maneira não-comercial, sem alterações e com atribuição ao autor.</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>84667</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>70556</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>762001</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>84667</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="Rectangle 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E4E24A3-6155-9C48-B422-C6E412817BE3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13405556" y="6194778"/>
-          <a:ext cx="4007556" cy="1792111"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Eu criei esse arquivo para ser usado gratuitamente. No entanto, se você sentir na sua alma que você quer me mandar 1000 reais pela graça alcançada, minha chave pix é meu email:</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>henriquefb arroba gmail ponto com</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -12500,7 +12430,9 @@
   </sheetPr>
   <dimension ref="D3:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
@@ -12552,7 +12484,7 @@
       <c r="Q41" s="16"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="xpce8UygQSah8zPj64ddaxTXvv/DTGzE/DGfEAMxfzDRN5ZKfdUDWmtwVOoHct+DMktM+4VR1nmAfOQ6pUvOqA==" saltValue="ZT2/ixGEffXDalCAG3HNng==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="mPOsBkPb5GlLmgz6uKDLpPnVtmfE3P1s+mlQs9y17D9vyAzkBLfnQJBxkUFG65AViu7iCG3YpWaFJIIt4HjfeQ==" saltValue="kfPI5IwN8gGkV0kzN5e/4Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -17942,51 +17874,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="81" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="81" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
     </row>
     <row r="3" spans="1:8" ht="16" customHeight="1">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="81" t="s">
         <v>115</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="82" t="s">
         <v>114</v>
       </c>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="81" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="74" t="s">
+      <c r="D3" s="81" t="s">
         <v>110</v>
       </c>
-      <c r="E3" s="74"/>
+      <c r="E3" s="81"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="74"/>
-      <c r="B4" s="76"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74" t="s">
+      <c r="A4" s="81"/>
+      <c r="B4" s="83"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="E4" s="74"/>
+      <c r="E4" s="81"/>
     </row>
     <row r="5" spans="1:8" ht="34" customHeight="1">
-      <c r="A5" s="74"/>
-      <c r="B5" s="77"/>
-      <c r="C5" s="74"/>
+      <c r="A5" s="81"/>
+      <c r="B5" s="84"/>
+      <c r="C5" s="81"/>
       <c r="D5" s="55" t="s">
         <v>107</v>
       </c>
@@ -18526,39 +18458,39 @@
       <c r="H32" s="58"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="72" t="s">
+      <c r="A33" s="79" t="s">
         <v>74</v>
       </c>
-      <c r="B33" s="72"/>
-      <c r="C33" s="72"/>
-      <c r="D33" s="72"/>
-      <c r="E33" s="72"/>
+      <c r="B33" s="79"/>
+      <c r="C33" s="79"/>
+      <c r="D33" s="79"/>
+      <c r="E33" s="79"/>
       <c r="G33" s="57" t="s">
         <v>89</v>
       </c>
       <c r="H33" s="58"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="73" t="s">
+      <c r="A34" s="80" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="73"/>
-      <c r="C34" s="73"/>
-      <c r="D34" s="73"/>
-      <c r="E34" s="73"/>
+      <c r="B34" s="80"/>
+      <c r="C34" s="80"/>
+      <c r="D34" s="80"/>
+      <c r="E34" s="80"/>
       <c r="G34" s="57" t="s">
         <v>82</v>
       </c>
       <c r="H34" s="58"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="72" t="s">
+      <c r="A35" s="79" t="s">
         <v>72</v>
       </c>
-      <c r="B35" s="72"/>
-      <c r="C35" s="72"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="72"/>
+      <c r="B35" s="79"/>
+      <c r="C35" s="79"/>
+      <c r="D35" s="79"/>
+      <c r="E35" s="79"/>
       <c r="G35" s="64" t="s">
         <v>76</v>
       </c>
@@ -18633,51 +18565,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="81" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="81" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
     </row>
     <row r="3" spans="1:8" ht="16" customHeight="1">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="81" t="s">
         <v>115</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="82" t="s">
         <v>114</v>
       </c>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="81" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="74" t="s">
+      <c r="D3" s="81" t="s">
         <v>110</v>
       </c>
-      <c r="E3" s="74"/>
+      <c r="E3" s="81"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="74"/>
-      <c r="B4" s="76"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74" t="s">
+      <c r="A4" s="81"/>
+      <c r="B4" s="83"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="E4" s="74"/>
+      <c r="E4" s="81"/>
     </row>
     <row r="5" spans="1:8" ht="34" customHeight="1">
-      <c r="A5" s="74"/>
-      <c r="B5" s="77"/>
-      <c r="C5" s="74"/>
+      <c r="A5" s="81"/>
+      <c r="B5" s="84"/>
+      <c r="C5" s="81"/>
       <c r="D5" s="55" t="s">
         <v>107</v>
       </c>
@@ -19259,13 +19191,13 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="72" t="s">
+      <c r="A33" s="79" t="s">
         <v>74</v>
       </c>
-      <c r="B33" s="72"/>
-      <c r="C33" s="72"/>
-      <c r="D33" s="72"/>
-      <c r="E33" s="72"/>
+      <c r="B33" s="79"/>
+      <c r="C33" s="79"/>
+      <c r="D33" s="79"/>
+      <c r="E33" s="79"/>
       <c r="G33" s="57" t="s">
         <v>89</v>
       </c>
@@ -19275,13 +19207,13 @@
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="73" t="s">
+      <c r="A34" s="80" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="73"/>
-      <c r="C34" s="73"/>
-      <c r="D34" s="73"/>
-      <c r="E34" s="73"/>
+      <c r="B34" s="80"/>
+      <c r="C34" s="80"/>
+      <c r="D34" s="80"/>
+      <c r="E34" s="80"/>
       <c r="G34" s="57" t="s">
         <v>82</v>
       </c>
@@ -19291,13 +19223,13 @@
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="72" t="s">
+      <c r="A35" s="79" t="s">
         <v>72</v>
       </c>
-      <c r="B35" s="72"/>
-      <c r="C35" s="72"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="72"/>
+      <c r="B35" s="79"/>
+      <c r="C35" s="79"/>
+      <c r="D35" s="79"/>
+      <c r="E35" s="79"/>
       <c r="G35" s="64" t="s">
         <v>76</v>
       </c>
@@ -19351,7 +19283,7 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="81" t="s">
+      <c r="A10" s="75" t="s">
         <v>131</v>
       </c>
       <c r="B10" t="s">
@@ -19363,7 +19295,7 @@
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="75" t="s">
         <v>132</v>
       </c>
       <c r="B11" t="s">
@@ -19375,7 +19307,7 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="81" t="s">
+      <c r="A12" s="75" t="s">
         <v>127</v>
       </c>
       <c r="C12" s="34" t="str">
@@ -19384,7 +19316,7 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="81" t="s">
+      <c r="A13" s="75" t="s">
         <v>130</v>
       </c>
       <c r="B13" t="s">
@@ -19396,7 +19328,7 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="81" t="s">
+      <c r="A14" s="75" t="s">
         <v>134</v>
       </c>
       <c r="B14" t="s">
@@ -19408,7 +19340,7 @@
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="81" t="s">
+      <c r="A15" s="75" t="s">
         <v>137</v>
       </c>
       <c r="B15" t="s">
@@ -19420,7 +19352,7 @@
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="81" t="s">
+      <c r="A16" s="75" t="s">
         <v>139</v>
       </c>
       <c r="B16" t="s">
@@ -19432,10 +19364,10 @@
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="81"/>
+      <c r="A17" s="75"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="81" t="s">
+      <c r="A19" s="75" t="s">
         <v>129</v>
       </c>
       <c r="B19">
@@ -19447,7 +19379,7 @@
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="81" t="s">
+      <c r="A20" s="75" t="s">
         <v>128</v>
       </c>
       <c r="B20">
@@ -19459,12 +19391,12 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="81" t="s">
+      <c r="A22" s="75" t="s">
         <v>133</v>
       </c>
-      <c r="C22" s="82">
+      <c r="C22" s="76">
         <f ca="1">NOW()</f>
-        <v>44477.443577777776</v>
+        <v>44481.752326388887</v>
       </c>
     </row>
   </sheetData>
@@ -19483,514 +19415,514 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="4" spans="3:17">
-      <c r="C4" s="83"/>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
-      <c r="K4" s="83"/>
-      <c r="L4" s="83"/>
-      <c r="M4" s="83"/>
-      <c r="N4" s="83"/>
-      <c r="O4" s="83"/>
-      <c r="P4" s="83"/>
-      <c r="Q4" s="83"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
+      <c r="K4" s="77"/>
+      <c r="L4" s="77"/>
+      <c r="M4" s="77"/>
+      <c r="N4" s="77"/>
+      <c r="O4" s="77"/>
+      <c r="P4" s="77"/>
+      <c r="Q4" s="77"/>
     </row>
     <row r="5" spans="3:17">
-      <c r="C5" s="83"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
-      <c r="L5" s="83"/>
-      <c r="M5" s="83"/>
-      <c r="N5" s="83"/>
-      <c r="O5" s="83"/>
-      <c r="P5" s="83"/>
-      <c r="Q5" s="83"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
+      <c r="L5" s="77"/>
+      <c r="M5" s="77"/>
+      <c r="N5" s="77"/>
+      <c r="O5" s="77"/>
+      <c r="P5" s="77"/>
+      <c r="Q5" s="77"/>
     </row>
     <row r="6" spans="3:17">
-      <c r="C6" s="83"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="84"/>
-      <c r="I6" s="84"/>
-      <c r="J6" s="84"/>
-      <c r="K6" s="84"/>
-      <c r="L6" s="84"/>
-      <c r="M6" s="84"/>
-      <c r="N6" s="84"/>
-      <c r="O6" s="84"/>
-      <c r="P6" s="84"/>
-      <c r="Q6" s="83"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="86"/>
+      <c r="L6" s="86"/>
+      <c r="M6" s="86"/>
+      <c r="N6" s="86"/>
+      <c r="O6" s="86"/>
+      <c r="P6" s="86"/>
+      <c r="Q6" s="77"/>
     </row>
     <row r="7" spans="3:17">
-      <c r="C7" s="83"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="84"/>
-      <c r="I7" s="84"/>
-      <c r="J7" s="84"/>
-      <c r="K7" s="84"/>
-      <c r="L7" s="84"/>
-      <c r="M7" s="84"/>
-      <c r="N7" s="84"/>
-      <c r="O7" s="84"/>
-      <c r="P7" s="84"/>
-      <c r="Q7" s="83"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="86"/>
+      <c r="L7" s="86"/>
+      <c r="M7" s="86"/>
+      <c r="N7" s="86"/>
+      <c r="O7" s="86"/>
+      <c r="P7" s="86"/>
+      <c r="Q7" s="77"/>
     </row>
     <row r="8" spans="3:17">
-      <c r="C8" s="83"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="84"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="84"/>
-      <c r="H8" s="84"/>
-      <c r="I8" s="84"/>
-      <c r="J8" s="84"/>
-      <c r="K8" s="84"/>
-      <c r="L8" s="84"/>
-      <c r="M8" s="84"/>
-      <c r="N8" s="84"/>
-      <c r="O8" s="84"/>
-      <c r="P8" s="84"/>
-      <c r="Q8" s="83"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="86"/>
+      <c r="J8" s="86"/>
+      <c r="K8" s="86"/>
+      <c r="L8" s="86"/>
+      <c r="M8" s="86"/>
+      <c r="N8" s="86"/>
+      <c r="O8" s="86"/>
+      <c r="P8" s="86"/>
+      <c r="Q8" s="77"/>
     </row>
     <row r="9" spans="3:17">
-      <c r="C9" s="83"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="84"/>
-      <c r="H9" s="84"/>
-      <c r="I9" s="84"/>
-      <c r="J9" s="84"/>
-      <c r="K9" s="84"/>
-      <c r="L9" s="84"/>
-      <c r="M9" s="84"/>
-      <c r="N9" s="84"/>
-      <c r="O9" s="84"/>
-      <c r="P9" s="84"/>
-      <c r="Q9" s="83"/>
+      <c r="C9" s="77"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="86"/>
+      <c r="G9" s="86"/>
+      <c r="H9" s="86"/>
+      <c r="I9" s="86"/>
+      <c r="J9" s="86"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="86"/>
+      <c r="M9" s="86"/>
+      <c r="N9" s="86"/>
+      <c r="O9" s="86"/>
+      <c r="P9" s="86"/>
+      <c r="Q9" s="77"/>
     </row>
     <row r="10" spans="3:17">
-      <c r="C10" s="83"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="84"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="84"/>
-      <c r="H10" s="84"/>
-      <c r="I10" s="84"/>
-      <c r="J10" s="84"/>
-      <c r="K10" s="84"/>
-      <c r="L10" s="84"/>
-      <c r="M10" s="84"/>
-      <c r="N10" s="84"/>
-      <c r="O10" s="84"/>
-      <c r="P10" s="84"/>
-      <c r="Q10" s="83"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="86"/>
+      <c r="G10" s="86"/>
+      <c r="H10" s="86"/>
+      <c r="I10" s="86"/>
+      <c r="J10" s="86"/>
+      <c r="K10" s="86"/>
+      <c r="L10" s="86"/>
+      <c r="M10" s="86"/>
+      <c r="N10" s="86"/>
+      <c r="O10" s="86"/>
+      <c r="P10" s="86"/>
+      <c r="Q10" s="77"/>
     </row>
     <row r="11" spans="3:17">
-      <c r="C11" s="83"/>
-      <c r="D11" s="83"/>
-      <c r="E11" s="83"/>
-      <c r="F11" s="83"/>
-      <c r="G11" s="83"/>
-      <c r="H11" s="83"/>
-      <c r="I11" s="83"/>
-      <c r="J11" s="83"/>
-      <c r="K11" s="83"/>
-      <c r="L11" s="83"/>
-      <c r="M11" s="83"/>
-      <c r="N11" s="83"/>
-      <c r="O11" s="83"/>
-      <c r="P11" s="83"/>
-      <c r="Q11" s="83"/>
+      <c r="C11" s="77"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="77"/>
+      <c r="H11" s="77"/>
+      <c r="I11" s="77"/>
+      <c r="J11" s="77"/>
+      <c r="K11" s="77"/>
+      <c r="L11" s="77"/>
+      <c r="M11" s="77"/>
+      <c r="N11" s="77"/>
+      <c r="O11" s="77"/>
+      <c r="P11" s="77"/>
+      <c r="Q11" s="77"/>
     </row>
     <row r="12" spans="3:17">
-      <c r="C12" s="83"/>
-      <c r="D12" s="83"/>
-      <c r="E12" s="83"/>
-      <c r="F12" s="83"/>
-      <c r="G12" s="83"/>
-      <c r="H12" s="83"/>
-      <c r="I12" s="83"/>
-      <c r="J12" s="83"/>
-      <c r="K12" s="83"/>
-      <c r="L12" s="83"/>
-      <c r="M12" s="83"/>
-      <c r="N12" s="83"/>
-      <c r="O12" s="83"/>
-      <c r="P12" s="83"/>
-      <c r="Q12" s="83"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="77"/>
+      <c r="H12" s="77"/>
+      <c r="I12" s="77"/>
+      <c r="J12" s="77"/>
+      <c r="K12" s="77"/>
+      <c r="L12" s="77"/>
+      <c r="M12" s="77"/>
+      <c r="N12" s="77"/>
+      <c r="O12" s="77"/>
+      <c r="P12" s="77"/>
+      <c r="Q12" s="77"/>
     </row>
     <row r="13" spans="3:17">
-      <c r="C13" s="83"/>
-      <c r="D13" s="83"/>
-      <c r="E13" s="83"/>
-      <c r="F13" s="83"/>
-      <c r="G13" s="83"/>
-      <c r="H13" s="83"/>
-      <c r="I13" s="83"/>
-      <c r="J13" s="83"/>
-      <c r="K13" s="83"/>
-      <c r="L13" s="83"/>
-      <c r="M13" s="83"/>
-      <c r="N13" s="83"/>
-      <c r="O13" s="83"/>
-      <c r="P13" s="83"/>
-      <c r="Q13" s="83"/>
+      <c r="C13" s="77"/>
+      <c r="D13" s="77"/>
+      <c r="E13" s="77"/>
+      <c r="F13" s="77"/>
+      <c r="G13" s="77"/>
+      <c r="H13" s="77"/>
+      <c r="I13" s="77"/>
+      <c r="J13" s="77"/>
+      <c r="K13" s="77"/>
+      <c r="L13" s="77"/>
+      <c r="M13" s="77"/>
+      <c r="N13" s="77"/>
+      <c r="O13" s="77"/>
+      <c r="P13" s="77"/>
+      <c r="Q13" s="77"/>
     </row>
     <row r="14" spans="3:17" ht="31">
-      <c r="C14" s="83"/>
-      <c r="D14" s="85"/>
-      <c r="E14" s="83"/>
-      <c r="F14" s="83"/>
-      <c r="G14" s="83"/>
-      <c r="H14" s="83"/>
-      <c r="I14" s="83"/>
-      <c r="J14" s="83"/>
-      <c r="K14" s="83"/>
-      <c r="L14" s="83"/>
-      <c r="M14" s="83"/>
-      <c r="N14" s="83"/>
-      <c r="O14" s="83"/>
-      <c r="P14" s="83"/>
-      <c r="Q14" s="83"/>
+      <c r="C14" s="77"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="77"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="77"/>
+      <c r="H14" s="77"/>
+      <c r="I14" s="77"/>
+      <c r="J14" s="77"/>
+      <c r="K14" s="77"/>
+      <c r="L14" s="77"/>
+      <c r="M14" s="77"/>
+      <c r="N14" s="77"/>
+      <c r="O14" s="77"/>
+      <c r="P14" s="77"/>
+      <c r="Q14" s="77"/>
     </row>
     <row r="15" spans="3:17">
-      <c r="C15" s="83"/>
-      <c r="D15" s="83"/>
-      <c r="E15" s="83"/>
-      <c r="F15" s="83"/>
-      <c r="G15" s="83"/>
-      <c r="H15" s="83"/>
-      <c r="I15" s="83"/>
-      <c r="J15" s="83"/>
-      <c r="K15" s="83"/>
-      <c r="L15" s="83"/>
-      <c r="M15" s="83"/>
-      <c r="N15" s="83"/>
-      <c r="O15" s="83"/>
-      <c r="P15" s="83"/>
-      <c r="Q15" s="83"/>
+      <c r="C15" s="77"/>
+      <c r="D15" s="77"/>
+      <c r="E15" s="77"/>
+      <c r="F15" s="77"/>
+      <c r="G15" s="77"/>
+      <c r="H15" s="77"/>
+      <c r="I15" s="77"/>
+      <c r="J15" s="77"/>
+      <c r="K15" s="77"/>
+      <c r="L15" s="77"/>
+      <c r="M15" s="77"/>
+      <c r="N15" s="77"/>
+      <c r="O15" s="77"/>
+      <c r="P15" s="77"/>
+      <c r="Q15" s="77"/>
     </row>
     <row r="16" spans="3:17">
-      <c r="C16" s="83"/>
-      <c r="D16" s="83"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="86"/>
-      <c r="G16" s="86"/>
-      <c r="H16" s="86"/>
-      <c r="I16" s="86"/>
-      <c r="J16" s="86"/>
-      <c r="K16" s="86"/>
-      <c r="L16" s="86"/>
-      <c r="M16" s="86"/>
-      <c r="N16" s="86"/>
-      <c r="O16" s="83"/>
-      <c r="P16" s="83"/>
-      <c r="Q16" s="83"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="77"/>
+      <c r="E16" s="87"/>
+      <c r="F16" s="87"/>
+      <c r="G16" s="87"/>
+      <c r="H16" s="87"/>
+      <c r="I16" s="87"/>
+      <c r="J16" s="87"/>
+      <c r="K16" s="87"/>
+      <c r="L16" s="87"/>
+      <c r="M16" s="87"/>
+      <c r="N16" s="87"/>
+      <c r="O16" s="77"/>
+      <c r="P16" s="77"/>
+      <c r="Q16" s="77"/>
     </row>
     <row r="17" spans="3:17">
-      <c r="C17" s="83"/>
-      <c r="D17" s="83"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="86"/>
-      <c r="G17" s="86"/>
-      <c r="H17" s="86"/>
-      <c r="I17" s="86"/>
-      <c r="J17" s="86"/>
-      <c r="K17" s="86"/>
-      <c r="L17" s="86"/>
-      <c r="M17" s="86"/>
-      <c r="N17" s="86"/>
-      <c r="O17" s="83"/>
-      <c r="P17" s="83"/>
-      <c r="Q17" s="83"/>
+      <c r="C17" s="77"/>
+      <c r="D17" s="77"/>
+      <c r="E17" s="87"/>
+      <c r="F17" s="87"/>
+      <c r="G17" s="87"/>
+      <c r="H17" s="87"/>
+      <c r="I17" s="87"/>
+      <c r="J17" s="87"/>
+      <c r="K17" s="87"/>
+      <c r="L17" s="87"/>
+      <c r="M17" s="87"/>
+      <c r="N17" s="87"/>
+      <c r="O17" s="77"/>
+      <c r="P17" s="77"/>
+      <c r="Q17" s="77"/>
     </row>
     <row r="18" spans="3:17">
-      <c r="C18" s="83"/>
-      <c r="D18" s="83"/>
-      <c r="E18" s="86"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="86"/>
-      <c r="H18" s="86"/>
-      <c r="I18" s="86"/>
-      <c r="J18" s="86"/>
-      <c r="K18" s="86"/>
-      <c r="L18" s="86"/>
-      <c r="M18" s="86"/>
-      <c r="N18" s="86"/>
-      <c r="O18" s="83"/>
-      <c r="P18" s="83"/>
-      <c r="Q18" s="83"/>
+      <c r="C18" s="77"/>
+      <c r="D18" s="77"/>
+      <c r="E18" s="87"/>
+      <c r="F18" s="87"/>
+      <c r="G18" s="87"/>
+      <c r="H18" s="87"/>
+      <c r="I18" s="87"/>
+      <c r="J18" s="87"/>
+      <c r="K18" s="87"/>
+      <c r="L18" s="87"/>
+      <c r="M18" s="87"/>
+      <c r="N18" s="87"/>
+      <c r="O18" s="77"/>
+      <c r="P18" s="77"/>
+      <c r="Q18" s="77"/>
     </row>
     <row r="19" spans="3:17">
-      <c r="C19" s="83"/>
-      <c r="D19" s="83"/>
-      <c r="E19" s="83"/>
-      <c r="F19" s="83"/>
-      <c r="G19" s="83"/>
-      <c r="H19" s="83"/>
-      <c r="I19" s="83"/>
-      <c r="J19" s="83"/>
-      <c r="K19" s="83"/>
-      <c r="L19" s="83"/>
-      <c r="M19" s="83"/>
-      <c r="N19" s="83"/>
-      <c r="O19" s="83"/>
-      <c r="P19" s="83"/>
-      <c r="Q19" s="83"/>
+      <c r="C19" s="77"/>
+      <c r="D19" s="77"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="77"/>
+      <c r="G19" s="77"/>
+      <c r="H19" s="77"/>
+      <c r="I19" s="77"/>
+      <c r="J19" s="77"/>
+      <c r="K19" s="77"/>
+      <c r="L19" s="77"/>
+      <c r="M19" s="77"/>
+      <c r="N19" s="77"/>
+      <c r="O19" s="77"/>
+      <c r="P19" s="77"/>
+      <c r="Q19" s="77"/>
     </row>
     <row r="20" spans="3:17">
-      <c r="C20" s="83"/>
-      <c r="D20" s="83"/>
-      <c r="E20" s="83"/>
-      <c r="F20" s="83"/>
-      <c r="G20" s="83"/>
-      <c r="H20" s="83"/>
-      <c r="I20" s="83"/>
-      <c r="J20" s="83"/>
-      <c r="K20" s="83"/>
-      <c r="L20" s="83"/>
-      <c r="M20" s="83"/>
-      <c r="N20" s="83"/>
-      <c r="O20" s="83"/>
-      <c r="P20" s="83"/>
-      <c r="Q20" s="83"/>
+      <c r="C20" s="77"/>
+      <c r="D20" s="77"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="77"/>
+      <c r="G20" s="77"/>
+      <c r="H20" s="77"/>
+      <c r="I20" s="77"/>
+      <c r="J20" s="77"/>
+      <c r="K20" s="77"/>
+      <c r="L20" s="77"/>
+      <c r="M20" s="77"/>
+      <c r="N20" s="77"/>
+      <c r="O20" s="77"/>
+      <c r="P20" s="77"/>
+      <c r="Q20" s="77"/>
     </row>
     <row r="21" spans="3:17" ht="33">
-      <c r="C21" s="83"/>
-      <c r="D21" s="87"/>
-      <c r="E21" s="87"/>
-      <c r="F21" s="87"/>
-      <c r="G21" s="87"/>
-      <c r="H21" s="87"/>
-      <c r="I21" s="87"/>
-      <c r="J21" s="87"/>
-      <c r="K21" s="87"/>
-      <c r="L21" s="87"/>
-      <c r="M21" s="87"/>
-      <c r="N21" s="87"/>
-      <c r="O21" s="87"/>
-      <c r="P21" s="83"/>
-      <c r="Q21" s="83"/>
+      <c r="C21" s="77"/>
+      <c r="D21" s="88"/>
+      <c r="E21" s="88"/>
+      <c r="F21" s="88"/>
+      <c r="G21" s="88"/>
+      <c r="H21" s="88"/>
+      <c r="I21" s="88"/>
+      <c r="J21" s="88"/>
+      <c r="K21" s="88"/>
+      <c r="L21" s="88"/>
+      <c r="M21" s="88"/>
+      <c r="N21" s="88"/>
+      <c r="O21" s="88"/>
+      <c r="P21" s="77"/>
+      <c r="Q21" s="77"/>
     </row>
     <row r="22" spans="3:17">
-      <c r="C22" s="83"/>
-      <c r="D22" s="83"/>
-      <c r="E22" s="83"/>
-      <c r="F22" s="83"/>
-      <c r="G22" s="83"/>
-      <c r="H22" s="83"/>
-      <c r="I22" s="83"/>
-      <c r="J22" s="83"/>
-      <c r="K22" s="83"/>
-      <c r="L22" s="83"/>
-      <c r="M22" s="83"/>
-      <c r="N22" s="83"/>
-      <c r="O22" s="83"/>
-      <c r="P22" s="83"/>
-      <c r="Q22" s="83"/>
+      <c r="C22" s="77"/>
+      <c r="D22" s="77"/>
+      <c r="E22" s="77"/>
+      <c r="F22" s="77"/>
+      <c r="G22" s="77"/>
+      <c r="H22" s="77"/>
+      <c r="I22" s="77"/>
+      <c r="J22" s="77"/>
+      <c r="K22" s="77"/>
+      <c r="L22" s="77"/>
+      <c r="M22" s="77"/>
+      <c r="N22" s="77"/>
+      <c r="O22" s="77"/>
+      <c r="P22" s="77"/>
+      <c r="Q22" s="77"/>
     </row>
     <row r="23" spans="3:17">
-      <c r="C23" s="83"/>
-      <c r="D23" s="83"/>
-      <c r="E23" s="83"/>
-      <c r="F23" s="83"/>
-      <c r="G23" s="83"/>
-      <c r="H23" s="83"/>
-      <c r="I23" s="83"/>
-      <c r="J23" s="83"/>
-      <c r="K23" s="83"/>
-      <c r="L23" s="83"/>
-      <c r="M23" s="83"/>
-      <c r="N23" s="83"/>
-      <c r="O23" s="83"/>
-      <c r="P23" s="83"/>
-      <c r="Q23" s="83"/>
+      <c r="C23" s="77"/>
+      <c r="D23" s="77"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="77"/>
+      <c r="G23" s="77"/>
+      <c r="H23" s="77"/>
+      <c r="I23" s="77"/>
+      <c r="J23" s="77"/>
+      <c r="K23" s="77"/>
+      <c r="L23" s="77"/>
+      <c r="M23" s="77"/>
+      <c r="N23" s="77"/>
+      <c r="O23" s="77"/>
+      <c r="P23" s="77"/>
+      <c r="Q23" s="77"/>
     </row>
     <row r="24" spans="3:17">
-      <c r="C24" s="83"/>
-      <c r="D24" s="83"/>
-      <c r="E24" s="83"/>
-      <c r="F24" s="83"/>
-      <c r="G24" s="83"/>
-      <c r="H24" s="83"/>
-      <c r="I24" s="83"/>
-      <c r="J24" s="83"/>
-      <c r="K24" s="83"/>
-      <c r="L24" s="83"/>
-      <c r="M24" s="83"/>
-      <c r="N24" s="83"/>
-      <c r="O24" s="83"/>
-      <c r="P24" s="83"/>
-      <c r="Q24" s="83"/>
+      <c r="C24" s="77"/>
+      <c r="D24" s="77"/>
+      <c r="E24" s="77"/>
+      <c r="F24" s="77"/>
+      <c r="G24" s="77"/>
+      <c r="H24" s="77"/>
+      <c r="I24" s="77"/>
+      <c r="J24" s="77"/>
+      <c r="K24" s="77"/>
+      <c r="L24" s="77"/>
+      <c r="M24" s="77"/>
+      <c r="N24" s="77"/>
+      <c r="O24" s="77"/>
+      <c r="P24" s="77"/>
+      <c r="Q24" s="77"/>
     </row>
     <row r="25" spans="3:17">
-      <c r="C25" s="83"/>
-      <c r="D25" s="83"/>
-      <c r="E25" s="83"/>
-      <c r="F25" s="83"/>
-      <c r="G25" s="83"/>
-      <c r="H25" s="83"/>
-      <c r="I25" s="83"/>
-      <c r="J25" s="83"/>
-      <c r="K25" s="83"/>
-      <c r="L25" s="83"/>
-      <c r="M25" s="83"/>
-      <c r="N25" s="83"/>
-      <c r="O25" s="83"/>
-      <c r="P25" s="83"/>
-      <c r="Q25" s="83"/>
+      <c r="C25" s="77"/>
+      <c r="D25" s="77"/>
+      <c r="E25" s="77"/>
+      <c r="F25" s="77"/>
+      <c r="G25" s="77"/>
+      <c r="H25" s="77"/>
+      <c r="I25" s="77"/>
+      <c r="J25" s="77"/>
+      <c r="K25" s="77"/>
+      <c r="L25" s="77"/>
+      <c r="M25" s="77"/>
+      <c r="N25" s="77"/>
+      <c r="O25" s="77"/>
+      <c r="P25" s="77"/>
+      <c r="Q25" s="77"/>
     </row>
     <row r="26" spans="3:17">
-      <c r="C26" s="83"/>
-      <c r="D26" s="83"/>
-      <c r="E26" s="83"/>
-      <c r="F26" s="83"/>
-      <c r="G26" s="83"/>
-      <c r="H26" s="83"/>
-      <c r="I26" s="83"/>
-      <c r="J26" s="83"/>
-      <c r="K26" s="83"/>
-      <c r="L26" s="83"/>
-      <c r="M26" s="83"/>
-      <c r="N26" s="83"/>
-      <c r="O26" s="83"/>
-      <c r="P26" s="83"/>
-      <c r="Q26" s="83"/>
+      <c r="C26" s="77"/>
+      <c r="D26" s="77"/>
+      <c r="E26" s="77"/>
+      <c r="F26" s="77"/>
+      <c r="G26" s="77"/>
+      <c r="H26" s="77"/>
+      <c r="I26" s="77"/>
+      <c r="J26" s="77"/>
+      <c r="K26" s="77"/>
+      <c r="L26" s="77"/>
+      <c r="M26" s="77"/>
+      <c r="N26" s="77"/>
+      <c r="O26" s="77"/>
+      <c r="P26" s="77"/>
+      <c r="Q26" s="77"/>
     </row>
     <row r="27" spans="3:17">
-      <c r="C27" s="83"/>
-      <c r="D27" s="83"/>
-      <c r="E27" s="83"/>
-      <c r="F27" s="83"/>
-      <c r="G27" s="83"/>
-      <c r="H27" s="83"/>
-      <c r="I27" s="83"/>
-      <c r="J27" s="83"/>
-      <c r="K27" s="83"/>
-      <c r="L27" s="83"/>
-      <c r="M27" s="83"/>
-      <c r="N27" s="83"/>
-      <c r="O27" s="83"/>
-      <c r="P27" s="83"/>
-      <c r="Q27" s="83"/>
+      <c r="C27" s="77"/>
+      <c r="D27" s="77"/>
+      <c r="E27" s="77"/>
+      <c r="F27" s="77"/>
+      <c r="G27" s="77"/>
+      <c r="H27" s="77"/>
+      <c r="I27" s="77"/>
+      <c r="J27" s="77"/>
+      <c r="K27" s="77"/>
+      <c r="L27" s="77"/>
+      <c r="M27" s="77"/>
+      <c r="N27" s="77"/>
+      <c r="O27" s="77"/>
+      <c r="P27" s="77"/>
+      <c r="Q27" s="77"/>
     </row>
     <row r="28" spans="3:17">
-      <c r="C28" s="83"/>
-      <c r="D28" s="83"/>
-      <c r="E28" s="83"/>
-      <c r="F28" s="83"/>
-      <c r="G28" s="83"/>
-      <c r="H28" s="83"/>
-      <c r="I28" s="83"/>
-      <c r="J28" s="83"/>
-      <c r="K28" s="83"/>
-      <c r="L28" s="83"/>
-      <c r="M28" s="83"/>
-      <c r="N28" s="83"/>
-      <c r="O28" s="83"/>
-      <c r="P28" s="83"/>
-      <c r="Q28" s="83"/>
+      <c r="C28" s="77"/>
+      <c r="D28" s="77"/>
+      <c r="E28" s="77"/>
+      <c r="F28" s="77"/>
+      <c r="G28" s="77"/>
+      <c r="H28" s="77"/>
+      <c r="I28" s="77"/>
+      <c r="J28" s="77"/>
+      <c r="K28" s="77"/>
+      <c r="L28" s="77"/>
+      <c r="M28" s="77"/>
+      <c r="N28" s="77"/>
+      <c r="O28" s="77"/>
+      <c r="P28" s="77"/>
+      <c r="Q28" s="77"/>
     </row>
     <row r="29" spans="3:17" ht="18">
-      <c r="C29" s="83"/>
-      <c r="D29" s="83"/>
-      <c r="E29" s="83"/>
-      <c r="F29" s="83"/>
-      <c r="G29" s="83"/>
-      <c r="H29" s="83"/>
-      <c r="I29" s="83"/>
-      <c r="J29" s="83"/>
-      <c r="K29" s="83"/>
-      <c r="L29" s="83"/>
-      <c r="M29" s="88"/>
-      <c r="N29" s="88"/>
-      <c r="O29" s="88"/>
-      <c r="P29" s="88"/>
-      <c r="Q29" s="83"/>
+      <c r="C29" s="77"/>
+      <c r="D29" s="77"/>
+      <c r="E29" s="77"/>
+      <c r="F29" s="77"/>
+      <c r="G29" s="77"/>
+      <c r="H29" s="77"/>
+      <c r="I29" s="77"/>
+      <c r="J29" s="77"/>
+      <c r="K29" s="77"/>
+      <c r="L29" s="77"/>
+      <c r="M29" s="89"/>
+      <c r="N29" s="89"/>
+      <c r="O29" s="89"/>
+      <c r="P29" s="89"/>
+      <c r="Q29" s="77"/>
     </row>
     <row r="30" spans="3:17">
-      <c r="C30" s="83"/>
-      <c r="D30" s="83"/>
-      <c r="E30" s="83"/>
-      <c r="F30" s="83"/>
-      <c r="G30" s="83"/>
-      <c r="H30" s="83"/>
-      <c r="I30" s="83"/>
-      <c r="J30" s="83"/>
-      <c r="K30" s="83"/>
-      <c r="L30" s="83"/>
-      <c r="M30" s="83"/>
-      <c r="N30" s="83"/>
-      <c r="O30" s="83"/>
-      <c r="P30" s="83"/>
-      <c r="Q30" s="83"/>
+      <c r="C30" s="77"/>
+      <c r="D30" s="77"/>
+      <c r="E30" s="77"/>
+      <c r="F30" s="77"/>
+      <c r="G30" s="77"/>
+      <c r="H30" s="77"/>
+      <c r="I30" s="77"/>
+      <c r="J30" s="77"/>
+      <c r="K30" s="77"/>
+      <c r="L30" s="77"/>
+      <c r="M30" s="77"/>
+      <c r="N30" s="77"/>
+      <c r="O30" s="77"/>
+      <c r="P30" s="77"/>
+      <c r="Q30" s="77"/>
     </row>
     <row r="31" spans="3:17">
-      <c r="C31" s="83"/>
-      <c r="D31" s="83"/>
-      <c r="E31" s="83"/>
-      <c r="F31" s="83"/>
-      <c r="G31" s="83"/>
-      <c r="H31" s="83"/>
-      <c r="I31" s="83"/>
-      <c r="J31" s="83"/>
-      <c r="K31" s="83"/>
-      <c r="L31" s="83"/>
-      <c r="M31" s="83"/>
-      <c r="N31" s="83"/>
-      <c r="O31" s="83"/>
-      <c r="P31" s="83"/>
-      <c r="Q31" s="83"/>
+      <c r="C31" s="77"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="77"/>
+      <c r="H31" s="77"/>
+      <c r="I31" s="77"/>
+      <c r="J31" s="77"/>
+      <c r="K31" s="77"/>
+      <c r="L31" s="77"/>
+      <c r="M31" s="77"/>
+      <c r="N31" s="77"/>
+      <c r="O31" s="77"/>
+      <c r="P31" s="77"/>
+      <c r="Q31" s="77"/>
     </row>
     <row r="32" spans="3:17">
-      <c r="C32" s="83"/>
-      <c r="D32" s="83"/>
-      <c r="E32" s="83"/>
-      <c r="F32" s="83"/>
-      <c r="G32" s="83"/>
-      <c r="H32" s="83"/>
-      <c r="I32" s="83"/>
-      <c r="J32" s="83"/>
-      <c r="K32" s="83"/>
-      <c r="L32" s="83"/>
-      <c r="M32" s="83"/>
-      <c r="N32" s="83"/>
-      <c r="O32" s="83"/>
-      <c r="P32" s="83"/>
-      <c r="Q32" s="83"/>
+      <c r="C32" s="77"/>
+      <c r="D32" s="77"/>
+      <c r="E32" s="77"/>
+      <c r="F32" s="77"/>
+      <c r="G32" s="77"/>
+      <c r="H32" s="77"/>
+      <c r="I32" s="77"/>
+      <c r="J32" s="77"/>
+      <c r="K32" s="77"/>
+      <c r="L32" s="77"/>
+      <c r="M32" s="77"/>
+      <c r="N32" s="77"/>
+      <c r="O32" s="77"/>
+      <c r="P32" s="77"/>
+      <c r="Q32" s="77"/>
     </row>
     <row r="33" spans="3:17">
-      <c r="C33" s="83"/>
-      <c r="D33" s="83"/>
-      <c r="E33" s="83"/>
-      <c r="F33" s="83"/>
-      <c r="G33" s="83"/>
-      <c r="H33" s="83"/>
-      <c r="I33" s="83"/>
-      <c r="J33" s="83"/>
-      <c r="K33" s="83"/>
-      <c r="L33" s="83"/>
-      <c r="M33" s="83"/>
-      <c r="N33" s="83"/>
-      <c r="O33" s="83"/>
-      <c r="P33" s="83"/>
-      <c r="Q33" s="83"/>
+      <c r="C33" s="77"/>
+      <c r="D33" s="77"/>
+      <c r="E33" s="77"/>
+      <c r="F33" s="77"/>
+      <c r="G33" s="77"/>
+      <c r="H33" s="77"/>
+      <c r="I33" s="77"/>
+      <c r="J33" s="77"/>
+      <c r="K33" s="77"/>
+      <c r="L33" s="77"/>
+      <c r="M33" s="77"/>
+      <c r="N33" s="77"/>
+      <c r="O33" s="77"/>
+      <c r="P33" s="77"/>
+      <c r="Q33" s="77"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="O0AhdGFdkIfKN1dnr5C6L3AAYXAvuXFZSFw84wsjuhqQ/GML7GRwGDbdVDArAuoP6vUW40RC/aRIdrwIzKwpFw==" saltValue="KxHte2mDl9W4+wq/Ktmxsg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
@@ -20228,7 +20160,7 @@
       <c r="M16" s="15"/>
     </row>
     <row r="17" spans="4:13">
-      <c r="D17" s="78">
+      <c r="D17" s="72">
         <f>SUM(E17:E18)</f>
         <v>15</v>
       </c>
@@ -22248,10 +22180,10 @@
       </c>
     </row>
     <row r="17" spans="13:14">
-      <c r="M17" s="79" t="s">
+      <c r="M17" s="73" t="s">
         <v>122</v>
       </c>
-      <c r="N17" s="80">
+      <c r="N17" s="74">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
mudança sutil de linguagem
</commit_message>
<xml_diff>
--- a/Aprenda Excel Usando Excel.xlsx
+++ b/Aprenda Excel Usando Excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/Documents/GitHub/AprendaExcelUsandoExcel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A88C3A-48A5-4546-B455-6268BAC6D563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94461FEB-449C-E449-8D74-8DC6402A1028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4640" yWindow="1840" windowWidth="28040" windowHeight="17440" xr2:uid="{BEAB5BE4-F684-DC48-92FB-55B2B06D943B}"/>
+    <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{BEAB5BE4-F684-DC48-92FB-55B2B06D943B}"/>
   </bookViews>
   <sheets>
     <sheet name="Apresentação" sheetId="1" r:id="rId1"/>
@@ -1293,7 +1293,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> Excel porque é meio intimidante. Tem várias coisas acontecendo, muitas fórmulas, e todo mundo que manja muito de Excel parece ser um mega NERD e VIRGEM. Mas você baixou esse tutorial porque você tá precisando de excel, e você não é NERD nem VIRGEM. Há esperança?</a:t>
+            <a:t> Excel porque é meio intimidante. Tem várias coisas acontecendo, muitas fórmulas, e todo mundo que manja muito de Excel parece ser um mega NERD. Mas você baixou esse tutorial porque você tá precisando de excel, e você não é um mega NERD. Há esperança?</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1363,7 +1363,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Boas notícias: Sim! Há esperança. Eu trabalho com Excel há mais de 10 anos (sim, sou nerd e virgem) e durante esse tempo eu entendi que em 95% do tempo a gente usa as mesmas 10 fórmulas. O pulo do gato é saber quais são essas fórmulas, QUANDO e COMO utilizá-las.</a:t>
+            <a:t>Boas notícias: Sim! Há esperança. Eu trabalho com Excel há mais de 10 anos (sim, sou um mega NERD) e durante esse tempo eu entendi que em 95% do tempo a gente usa as mesmas 10 fórmulas. O pulo do gato é saber quais são essas fórmulas, QUANDO e COMO utilizá-las.</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -12431,7 +12431,7 @@
   <dimension ref="D3:Q41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -12484,7 +12484,7 @@
       <c r="Q41" s="16"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="mPOsBkPb5GlLmgz6uKDLpPnVtmfE3P1s+mlQs9y17D9vyAzkBLfnQJBxkUFG65AViu7iCG3YpWaFJIIt4HjfeQ==" saltValue="kfPI5IwN8gGkV0kzN5e/4Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Tcgo2d9moJ4IEh2NuHUkq1bmwCLx3QCY06I8BVTKSkWj5C7T+/sAJ/3yN2jS6epovjOOrRl7C+PzzdvuEAmm5Q==" saltValue="bf2aYJ6A8K2/RG4HPBTrKg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -19396,7 +19396,7 @@
       </c>
       <c r="C22" s="76">
         <f ca="1">NOW()</f>
-        <v>44481.752326388887</v>
+        <v>44544.56000046296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>